<commit_message>
Fixed some tables and figures
</commit_message>
<xml_diff>
--- a/results/output/recall.city.populated.xlsx
+++ b/results/output/recall.city.populated.xlsx
@@ -2075,7 +2075,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="AL9" t="n">
-        <v>0.6666666666666666</v>
+        <v>1.0</v>
       </c>
       <c r="AM9" t="n">
         <v>0.16666666666666666</v>
@@ -2432,7 +2432,7 @@
         <v>0.0</v>
       </c>
       <c r="AL12" t="n">
-        <v>0.6666666666666666</v>
+        <v>1.0</v>
       </c>
       <c r="AM12" t="n">
         <v>0.0</v>
@@ -2551,7 +2551,7 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="AL13" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AM13" t="n">
         <v>0.3333333333333333</v>
@@ -3384,7 +3384,7 @@
         <v>0.5</v>
       </c>
       <c r="AL20" t="n">
-        <v>0.6666666666666666</v>
+        <v>1.0</v>
       </c>
       <c r="AM20" t="n">
         <v>0.5</v>
@@ -3741,7 +3741,7 @@
         <v>0.5</v>
       </c>
       <c r="AL23" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AM23" t="n">
         <v>0.5</v>
@@ -3860,7 +3860,7 @@
         <v>0.0</v>
       </c>
       <c r="AL24" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AM24" t="n">
         <v>0.0</v>
@@ -6359,7 +6359,7 @@
         <v>0.0</v>
       </c>
       <c r="AL45" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AM45" t="n">
         <v>0.0</v>
@@ -6835,7 +6835,7 @@
         <v>0.0</v>
       </c>
       <c r="AL49" t="n">
-        <v>1.0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AM49" t="n">
         <v>0.0</v>
@@ -9334,7 +9334,7 @@
         <v>0.0</v>
       </c>
       <c r="AL70" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AM70" t="n">
         <v>0.0</v>
@@ -9453,7 +9453,7 @@
         <v>0.0</v>
       </c>
       <c r="AL71" t="n">
-        <v>0.6666666666666666</v>
+        <v>1.0</v>
       </c>
       <c r="AM71" t="n">
         <v>0.0</v>
@@ -9572,7 +9572,7 @@
         <v>0.0</v>
       </c>
       <c r="AL72" t="n">
-        <v>0.6666666666666666</v>
+        <v>1.0</v>
       </c>
       <c r="AM72" t="n">
         <v>0.0</v>
@@ -10286,7 +10286,7 @@
         <v>0.25</v>
       </c>
       <c r="AL78" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AM78" t="n">
         <v>0.25</v>

</xml_diff>

<commit_message>
Added simulations; anonymized files
</commit_message>
<xml_diff>
--- a/results/output/recall.city.populated.xlsx
+++ b/results/output/recall.city.populated.xlsx
@@ -2271,7 +2271,7 @@
         <v>0.0</v>
       </c>
       <c r="AL11" t="n">
-        <v>0.6666666666666666</v>
+        <v>1.0</v>
       </c>
       <c r="AM11" t="n">
         <v>0.0</v>
@@ -2390,7 +2390,7 @@
         <v>0.3333333333333333</v>
       </c>
       <c r="AL12" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="AM12" t="n">
         <v>0.3333333333333333</v>
@@ -3223,7 +3223,7 @@
         <v>0.5</v>
       </c>
       <c r="AL19" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AM19" t="n">
         <v>0.5</v>
@@ -5960,7 +5960,7 @@
         <v>0.0</v>
       </c>
       <c r="AL42" t="n">
-        <v>0.6666666666666666</v>
+        <v>1.0</v>
       </c>
       <c r="AM42" t="n">
         <v>0.0</v>
@@ -6079,7 +6079,7 @@
         <v>0.0</v>
       </c>
       <c r="AL43" t="n">
-        <v>0.6666666666666666</v>
+        <v>1.0</v>
       </c>
       <c r="AM43" t="n">
         <v>0.0</v>
@@ -6555,7 +6555,7 @@
         <v>0.0</v>
       </c>
       <c r="AL47" t="n">
-        <v>0.3333333333333333</v>
+        <v>1.0</v>
       </c>
       <c r="AM47" t="n">
         <v>0.0</v>
@@ -13814,7 +13814,7 @@
         <v>0.0</v>
       </c>
       <c r="AL108" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AM108" t="n">
         <v>0.0</v>

</xml_diff>